<commit_message>
Optimized __get_list_of_games to vastly minimize linear searches through the entiry of the gamelog. Result: 6 second, or 20 %, average speed increase
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17020" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="19140" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="After _check_year opt" sheetId="1" r:id="rId1"/>
-    <sheet name="After listOfGames Opt1" sheetId="2" r:id="rId2"/>
+    <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
+    <sheet name="listOfGames Opt1" sheetId="2" r:id="rId2"/>
+    <sheet name=" listOfGames Opt2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t>T1</t>
   </si>
@@ -103,22 +104,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -581,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -597,7 +604,7 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -612,11 +619,11 @@
         <v>33.917000000000002</v>
       </c>
       <c r="D2">
-        <v>60.448999999999998</v>
-      </c>
-      <c r="E2">
+        <v>34.156999999999996</v>
+      </c>
+      <c r="E2" s="3">
         <f>AVERAGE(B2:D2)</f>
-        <v>42.720666666666659</v>
+        <v>33.956666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -630,11 +637,11 @@
         <v>32.857999999999997</v>
       </c>
       <c r="D3">
-        <v>53.780999999999999</v>
-      </c>
-      <c r="E3">
+        <v>33.08</v>
+      </c>
+      <c r="E3" s="3">
         <f>AVERAGE(B3:D3)</f>
-        <v>39.786999999999999</v>
+        <v>32.886666666666663</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -648,11 +655,11 @@
         <v>1.0529999999999999</v>
       </c>
       <c r="D4">
-        <v>6.6559999999999997</v>
-      </c>
-      <c r="E4">
+        <v>1.07</v>
+      </c>
+      <c r="E4" s="3">
         <f>AVERAGE(B4:D4)</f>
-        <v>2.9236666666666671</v>
+        <v>1.0616666666666668</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -669,11 +676,11 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>60.436999999999998</v>
-      </c>
-      <c r="E5">
+        <v>34.15</v>
+      </c>
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>42.710666666666668</v>
+        <v>33.948333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -690,11 +697,142 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
+        <v>6.9999999999978968E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3333333333328596E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>33.795999999999999</v>
+      </c>
+      <c r="C2">
+        <v>33.917000000000002</v>
+      </c>
+      <c r="D2">
+        <v>34.156999999999996</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>33.956666666666663</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>32.722000000000001</v>
+      </c>
+      <c r="C3">
+        <v>32.857999999999997</v>
+      </c>
+      <c r="D3">
+        <v>33.08</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>32.886666666666663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1.0620000000000001</v>
+      </c>
+      <c r="C4">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="D4">
+        <v>1.07</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>1.0616666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>33.783999999999999</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>33.910999999999994</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>34.15</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>33.948333333333331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
         <v>1.2000000000000455E-2</v>
       </c>
-      <c r="E6">
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>6.0000000000073328E-3</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="1"/>
-        <v>9.9999999999909051E-3</v>
+        <v>6.9999999999978968E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3333333333328596E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimized get participants to return a generator instead of a list
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="23360" windowHeight="15560" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="16280" windowHeight="15560" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
     <sheet name="listOfGames Opt1" sheetId="2" r:id="rId2"/>
     <sheet name=" listOfGames Opt2" sheetId="3" r:id="rId3"/>
+    <sheet name="get_participants Opt1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
   <si>
     <t>T1</t>
   </si>
@@ -48,6 +49,9 @@
   </si>
   <si>
     <t>R - (U+S)</t>
+  </si>
+  <si>
+    <t>Note: This was after first making the changes. For some reason, the next morning all the timings are coming out around 33 seconds..</t>
   </si>
 </sst>
 </file>
@@ -104,8 +108,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -119,13 +125,15 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -717,10 +725,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -833,6 +841,142 @@
       <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>0.58433333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>28.92</v>
+      </c>
+      <c r="C2">
+        <v>28.48</v>
+      </c>
+      <c r="D2">
+        <v>28.481000000000002</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>28.626999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>27.951000000000001</v>
+      </c>
+      <c r="C3">
+        <v>27.878</v>
+      </c>
+      <c r="D3">
+        <v>27.512</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>27.780333333333335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="C4">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="D4">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>28.913</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>28.832000000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>28.471</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>28.738666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>7.0000000000014495E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>-0.35200000000000031</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.0000000000001563E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.11166666666666814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made get_participants simply check len instead of use a regular expression. 5 second speed improvement
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="16280" windowHeight="15560" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="16280" windowHeight="15560" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
     <sheet name="listOfGames Opt1" sheetId="2" r:id="rId2"/>
     <sheet name=" listOfGames Opt2" sheetId="3" r:id="rId3"/>
     <sheet name="get_participants Opt1" sheetId="4" r:id="rId4"/>
+    <sheet name="get_participants_Opt1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
   <si>
     <t>T1</t>
   </si>
@@ -108,8 +109,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -125,15 +128,17 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -863,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -977,6 +982,137 @@
       <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>-0.11166666666666814</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>26.111999999999998</v>
+      </c>
+      <c r="C2">
+        <v>20.936</v>
+      </c>
+      <c r="D2">
+        <v>22.914000000000001</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>23.320666666666668</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>22.207000000000001</v>
+      </c>
+      <c r="C3">
+        <v>19.952000000000002</v>
+      </c>
+      <c r="D3">
+        <v>21.914999999999999</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>21.358000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>1.3169999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="D4">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>1.095</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>23.524000000000001</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>20.931000000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>22.904</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>22.453000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>2.5879999999999974</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>4.9999999999990052E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.0000000000001563E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.86766666666666481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created a playerInfo buffer to reduce unnecessary did_get_hit calculations. Cut 10 seconds off
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="16280" windowHeight="15560" tabRatio="500" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="19300" windowHeight="15560" tabRatio="500" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name=" listOfGames Opt2" sheetId="3" r:id="rId3"/>
     <sheet name="get_participants Opt1" sheetId="4" r:id="rId4"/>
     <sheet name="get_participants_Opt1" sheetId="5" r:id="rId5"/>
+    <sheet name="_search_boxscore Opt1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="11">
   <si>
     <t>T1</t>
   </si>
@@ -54,12 +55,15 @@
   <si>
     <t>Note: This was after first making the changes. For some reason, the next morning all the timings are coming out around 33 seconds..</t>
   </si>
+  <si>
+    <t xml:space="preserve">Date: </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +95,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -109,7 +128,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -121,24 +140,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -468,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="A1:E6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,8 +527,11 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -507,8 +548,11 @@
         <f>AVERAGE(B2:D2)</f>
         <v>60.997333333333337</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="4">
+        <v>41800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -526,7 +570,7 @@
         <v>53.943999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -544,7 +588,7 @@
         <v>6.6676666666666664</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -565,7 +609,7 @@
         <v>60.611666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -599,15 +643,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="A1:E6"/>
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,8 +664,11 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -638,8 +685,11 @@
         <f>AVERAGE(B2:D2)</f>
         <v>33.956666666666663</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="4">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -657,7 +707,7 @@
         <v>32.886666666666663</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -675,7 +725,7 @@
         <v>1.0616666666666668</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -696,7 +746,7 @@
         <v>33.948333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -730,15 +780,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -769,8 +819,11 @@
         <f>AVERAGE(B2:D2)</f>
         <v>27.480333333333334</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -787,8 +840,11 @@
         <f>AVERAGE(B3:D3)</f>
         <v>25.968333333333334</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" s="4">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -806,7 +862,7 @@
         <v>0.92766666666666653</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -827,7 +883,7 @@
         <v>26.896000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -848,7 +904,7 @@
         <v>0.58433333333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -866,15 +922,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="A1:E6"/>
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -887,8 +943,11 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -905,8 +964,11 @@
         <f>AVERAGE(B2:D2)</f>
         <v>28.626999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="6">
+        <v>41802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -924,7 +986,7 @@
         <v>27.780333333333335</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -942,7 +1004,7 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -963,7 +1025,7 @@
         <v>28.738666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -997,15 +1059,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1018,8 +1080,11 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1036,8 +1101,11 @@
         <f>AVERAGE(B2:D2)</f>
         <v>23.320666666666668</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="6">
+        <v>41802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1055,7 +1123,7 @@
         <v>21.358000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1073,7 +1141,7 @@
         <v>1.095</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1094,7 +1162,7 @@
         <v>22.453000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1113,6 +1181,143 @@
       <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>0.86766666666666481</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>19.297999999999998</v>
+      </c>
+      <c r="C2">
+        <v>17.789000000000001</v>
+      </c>
+      <c r="D2">
+        <v>17.834</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>18.307000000000002</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="C3">
+        <v>16.853000000000002</v>
+      </c>
+      <c r="D3">
+        <v>16.896999999999998</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>17.366666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="C4">
+        <v>0.93</v>
+      </c>
+      <c r="D4">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.93066666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>19.279</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>17.783000000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>17.829999999999998</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>18.297333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>1.8999999999998352E-2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>6.0000000000002274E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4.0000000000013358E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>9.6666666666678225E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed progressbar from get_playres
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="19300" windowHeight="15560" tabRatio="500" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="19300" windowHeight="15560" tabRatio="500" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="get_participants Opt1" sheetId="4" r:id="rId4"/>
     <sheet name="get_participants_Opt1" sheetId="5" r:id="rId5"/>
     <sheet name="_search_boxscore Opt1" sheetId="6" r:id="rId6"/>
+    <sheet name="introduced playerInfoBuffer" sheetId="7" r:id="rId7"/>
+    <sheet name="Killed get_players progressbar" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="11">
   <si>
     <t>T1</t>
   </si>
@@ -128,8 +130,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -158,7 +164,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -168,6 +174,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -177,6 +185,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1198,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1318,6 +1328,280 @@
       <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>9.6666666666678225E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>8.4019999999999992</v>
+      </c>
+      <c r="C2">
+        <v>8.3119999999999994</v>
+      </c>
+      <c r="D2">
+        <v>8.3629999999999995</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>8.359</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.6470000000000002</v>
+      </c>
+      <c r="C3">
+        <v>7.569</v>
+      </c>
+      <c r="D3">
+        <v>7.6050000000000004</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>7.6070000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.751</v>
+      </c>
+      <c r="C4">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="D4">
+        <v>0.754</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.74799999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>8.3979999999999997</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>8.3079999999999998</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8.359</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>8.3550000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>3.9999999999995595E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>3.9999999999995595E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>3.9999999999995595E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.9999999999995595E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>8.31</v>
+      </c>
+      <c r="C2">
+        <v>8.2520000000000007</v>
+      </c>
+      <c r="D2">
+        <v>8.33</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>8.2973333333333343</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.556</v>
+      </c>
+      <c r="C3">
+        <v>7.4989999999999997</v>
+      </c>
+      <c r="D3">
+        <v>7.585</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>7.5466666666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.751</v>
+      </c>
+      <c r="C4">
+        <v>0.749</v>
+      </c>
+      <c r="D4">
+        <v>0.74</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.7466666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>8.3070000000000004</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>8.2479999999999993</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8.3249999999999993</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>8.293333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>3.0000000000001137E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>4.0000000000013358E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>5.0000000000007816E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>4.0000000000013358E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed indices from players
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="19300" windowHeight="15560" tabRatio="500" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="19300" windowHeight="15560" tabRatio="500" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="_search_boxscore Opt1" sheetId="6" r:id="rId6"/>
     <sheet name="introduced playerInfoBuffer" sheetId="7" r:id="rId7"/>
     <sheet name="Killed get_players progressbar" sheetId="8" r:id="rId8"/>
+    <sheet name="Removed Index from Player " sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="11">
   <si>
     <t>T1</t>
   </si>
@@ -130,8 +131,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -164,7 +167,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -176,6 +179,7 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -187,6 +191,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1482,6 +1487,143 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>8.31</v>
+      </c>
+      <c r="C2">
+        <v>8.2520000000000007</v>
+      </c>
+      <c r="D2">
+        <v>8.33</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>8.2973333333333343</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.556</v>
+      </c>
+      <c r="C3">
+        <v>7.4989999999999997</v>
+      </c>
+      <c r="D3">
+        <v>7.585</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>7.5466666666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.751</v>
+      </c>
+      <c r="C4">
+        <v>0.749</v>
+      </c>
+      <c r="D4">
+        <v>0.74</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.7466666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>8.3070000000000004</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>8.2479999999999993</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8.3249999999999993</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>8.293333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>3.0000000000001137E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>4.0000000000013358E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>5.0000000000007816E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>4.0000000000013358E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
@@ -1510,17 +1652,17 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>8.31</v>
+        <v>8.1549999999999994</v>
       </c>
       <c r="C2">
-        <v>8.2520000000000007</v>
+        <v>8.407</v>
       </c>
       <c r="D2">
-        <v>8.33</v>
+        <v>8.2449999999999992</v>
       </c>
       <c r="E2" s="3">
         <f>AVERAGE(B2:D2)</f>
-        <v>8.2973333333333343</v>
+        <v>8.2689999999999984</v>
       </c>
       <c r="G2" s="6">
         <v>41802</v>
@@ -1531,17 +1673,17 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>7.556</v>
+        <v>7.415</v>
       </c>
       <c r="C3">
-        <v>7.4989999999999997</v>
+        <v>7.6440000000000001</v>
       </c>
       <c r="D3">
-        <v>7.585</v>
+        <v>7.5049999999999999</v>
       </c>
       <c r="E3" s="3">
         <f>AVERAGE(B3:D3)</f>
-        <v>7.5466666666666669</v>
+        <v>7.5213333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1549,17 +1691,17 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.751</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="C4">
-        <v>0.749</v>
+        <v>0.746</v>
       </c>
       <c r="D4">
-        <v>0.74</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="E4" s="3">
         <f>AVERAGE(B4:D4)</f>
-        <v>0.7466666666666667</v>
+        <v>0.73966666666666681</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1568,19 +1710,19 @@
       </c>
       <c r="B5">
         <f>SUM(B3:B4)</f>
-        <v>8.3070000000000004</v>
+        <v>8.1519999999999992</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
-        <v>8.2479999999999993</v>
+        <v>8.39</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>8.3249999999999993</v>
+        <v>8.2409999999999997</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>8.293333333333333</v>
+        <v>8.261000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1593,15 +1735,15 @@
       </c>
       <c r="C6">
         <f t="shared" ref="C6:E6" si="1">C2-C5</f>
-        <v>4.0000000000013358E-3</v>
+        <v>1.699999999999946E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>5.0000000000007816E-3</v>
+        <v>3.9999999999995595E-3</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="1"/>
-        <v>4.0000000000013358E-3</v>
+        <v>7.9999999999973426E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fully installed bot update buffer.
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="19300" windowHeight="15560" tabRatio="500" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="19300" windowHeight="15560" tabRatio="500" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="introduced playerInfoBuffer" sheetId="7" r:id="rId7"/>
     <sheet name="Killed get_players progressbar" sheetId="8" r:id="rId8"/>
     <sheet name="Removed Index from Player " sheetId="9" r:id="rId9"/>
+    <sheet name="Created update_history buffer" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="11">
   <si>
     <t>T1</t>
   </si>
@@ -131,8 +132,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -167,7 +172,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -180,6 +185,8 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -192,6 +199,8 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -656,6 +665,142 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>8.1639999999999997</v>
+      </c>
+      <c r="C2">
+        <v>7.9939999999999998</v>
+      </c>
+      <c r="D2">
+        <v>8.0190000000000001</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>8.0589999999999993</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41802</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.4420000000000002</v>
+      </c>
+      <c r="C3">
+        <v>7.266</v>
+      </c>
+      <c r="D3">
+        <v>7.2930000000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>7.3336666666666668</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="D4">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.72366666666666679</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>8.1669999999999998</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>7.9879999999999995</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8.0169999999999995</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>8.0573333333333341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>-3.0000000000001137E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>6.0000000000002274E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>2.0000000000006679E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6666666666651508E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
@@ -1624,8 +1769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1748,6 +1893,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
100% test coverage for researcher, including all memoization buffers
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="19300" windowHeight="15560" tabRatio="500" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="Killed get_players progressbar" sheetId="8" r:id="rId8"/>
     <sheet name="Removed Index from Player " sheetId="9" r:id="rId9"/>
     <sheet name="Created update_history buffer" sheetId="10" r:id="rId10"/>
+    <sheet name="Fixed playerInfo appends" sheetId="11" r:id="rId11"/>
+    <sheet name="Switched to iTerm2" sheetId="12" r:id="rId12"/>
+    <sheet name="Change to boxscoreBuffer" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="15">
   <si>
     <t>T1</t>
   </si>
@@ -61,6 +64,18 @@
   </si>
   <si>
     <t xml:space="preserve">Date: </t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>Switched from testing in terminal</t>
+  </si>
+  <si>
+    <t>to testing in iTerm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduced dictionary lookups in boxscore buffer by 33%ish. </t>
   </si>
 </sst>
 </file>
@@ -132,8 +147,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -172,7 +201,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -187,6 +216,13 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -201,6 +237,13 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -669,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -793,6 +836,434 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>7.8789999999999996</v>
+      </c>
+      <c r="C2">
+        <v>7.7649999999999997</v>
+      </c>
+      <c r="D2">
+        <v>8.0229999999999997</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>7.8889999999999993</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.1550000000000002</v>
+      </c>
+      <c r="C3">
+        <v>7.0510000000000002</v>
+      </c>
+      <c r="D3">
+        <v>7.2960000000000003</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>7.1673333333333327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.72</v>
+      </c>
+      <c r="C4">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="D4">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.71766666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>7.875</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>7.7590000000000003</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8.0210000000000008</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>7.8849999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>3.9999999999995595E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>5.9999999999993392E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.9999999999988916E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.9999999999995595E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>8.0250000000000004</v>
+      </c>
+      <c r="C2">
+        <v>7.8570000000000002</v>
+      </c>
+      <c r="D2">
+        <v>7.8369999999999997</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>7.9063333333333334</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41809</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.1479999999999997</v>
+      </c>
+      <c r="C3">
+        <v>7.1219999999999999</v>
+      </c>
+      <c r="D3">
+        <v>7.1239999999999997</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>7.1313333333333331</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.73</v>
+      </c>
+      <c r="D4">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.72199999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>7.8759999999999994</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>7.8520000000000003</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.8319999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>7.8533333333333335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>0.14900000000000091</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>5.2999999999999936E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>7.9889999999999999</v>
+      </c>
+      <c r="C2">
+        <v>7.7809999999999997</v>
+      </c>
+      <c r="D2">
+        <v>7.9649999999999999</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>7.9116666666666662</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41809</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.2560000000000002</v>
+      </c>
+      <c r="C3">
+        <v>7.0609999999999999</v>
+      </c>
+      <c r="D3">
+        <v>7.2359999999999998</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>7.1843333333333339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="D4">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.72266666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>7.984</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>7.7770000000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.96</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>7.9070000000000009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>3.9999999999995595E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>4.6666666666652645E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Successfully created an experimental C extension named experiment
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500" firstSheet="11" activeTab="12"/>
+    <workbookView xWindow="2000" yWindow="0" windowWidth="11120" windowHeight="15380" tabRatio="500" firstSheet="13" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Fixed playerInfo appends" sheetId="11" r:id="rId11"/>
     <sheet name="Switched to iTerm2" sheetId="12" r:id="rId12"/>
     <sheet name="Change to boxscoreBuffer" sheetId="13" r:id="rId13"/>
+    <sheet name="Mass simulation working" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="16">
   <si>
     <t>T1</t>
   </si>
@@ -76,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">reduced dictionary lookups in boxscore buffer by 33%ish. </t>
+  </si>
+  <si>
+    <t>Did not reduce lines of code used explicitly for testing</t>
   </si>
 </sst>
 </file>
@@ -147,8 +151,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -201,7 +207,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -223,6 +229,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -244,6 +251,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1133,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1264,6 +1272,148 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>7.9429999999999996</v>
+      </c>
+      <c r="C2">
+        <v>7.7220000000000004</v>
+      </c>
+      <c r="D2">
+        <v>7.9359999999999999</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>7.867</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41810</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>7.2279999999999998</v>
+      </c>
+      <c r="C3">
+        <v>7.0129999999999999</v>
+      </c>
+      <c r="D3">
+        <v>7.21</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>7.1503333333333332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="C4">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="D4">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.71233333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>7.9369999999999994</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>7.72</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.931</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>7.8626666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>6.0000000000002274E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>2.0000000000006679E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>4.3333333333333002E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
About to refactor cresearcher to reduce repeated logic
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="0" windowWidth="11120" windowHeight="15380" tabRatio="500" firstSheet="13" activeTab="13"/>
+    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Switched to iTerm2" sheetId="12" r:id="rId12"/>
     <sheet name="Change to boxscoreBuffer" sheetId="13" r:id="rId13"/>
     <sheet name="Mass simulation working" sheetId="14" r:id="rId14"/>
+    <sheet name="created c_did_get_hit" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="17">
   <si>
     <t>T1</t>
   </si>
@@ -80,6 +81,9 @@
   </si>
   <si>
     <t>Did not reduce lines of code used explicitly for testing</t>
+  </si>
+  <si>
+    <t>% Improvement</t>
   </si>
 </sst>
 </file>
@@ -151,8 +155,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -207,7 +213,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -230,6 +236,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -252,6 +259,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1284,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1410,6 +1418,164 @@
       <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>4.3333333333333002E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>6.1669999999999998</v>
+      </c>
+      <c r="C2">
+        <v>6.1609999999999996</v>
+      </c>
+      <c r="D2">
+        <v>6.1269999999999998</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>6.1516666666666664</v>
+      </c>
+      <c r="F2" s="3">
+        <f>('Mass simulation working'!E2-'created c_did_get_hit'!E2)/'Mass simulation working'!E2</f>
+        <v>0.2180416084064235</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41811</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5.4649999999999999</v>
+      </c>
+      <c r="C3">
+        <v>5.468</v>
+      </c>
+      <c r="D3">
+        <v>5.4409999999999998</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>5.4579999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="C4">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="D4">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>6.1619999999999999</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>6.157</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>6.125</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>6.1479999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>4.9999999999998934E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>3.9999999999995595E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.9999999999997797E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.6666666666667069E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed redundant batAve calcs in setup
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="13" activeTab="14"/>
+    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="14" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="Change to boxscoreBuffer" sheetId="13" r:id="rId13"/>
     <sheet name="Mass simulation working" sheetId="14" r:id="rId14"/>
     <sheet name="created c_did_get_hit" sheetId="15" r:id="rId15"/>
+    <sheet name="optimized rId in participants" sheetId="16" r:id="rId16"/>
+    <sheet name="no redun batAve calcs" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="22">
   <si>
     <t>T1</t>
   </si>
@@ -84,6 +86,21 @@
   </si>
   <si>
     <t>% Improvement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We're now returning a set instead of a generator from get_participants, </t>
+  </si>
+  <si>
+    <t>which allows for hash-based lookups</t>
+  </si>
+  <si>
+    <t>Setup was having the players calculate their batting averages again…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">even though the batave csvs have that info!! </t>
+  </si>
+  <si>
+    <t>Dumb.</t>
   </si>
 </sst>
 </file>
@@ -155,8 +172,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,7 +234,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -237,6 +258,8 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -260,6 +283,8 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1435,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1576,6 +1601,321 @@
       <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>3.6666666666667069E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="A1:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>5.6120000000000001</v>
+      </c>
+      <c r="C2">
+        <v>5.7329999999999997</v>
+      </c>
+      <c r="D2">
+        <v>5.6630000000000003</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>5.6693333333333333</v>
+      </c>
+      <c r="F2" s="3">
+        <f>('created c_did_get_hit'!E2 - E2)/'created c_did_get_hit'!E2</f>
+        <v>7.8406935789758825E-2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41811</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>4.9240000000000004</v>
+      </c>
+      <c r="C3">
+        <v>5.0359999999999996</v>
+      </c>
+      <c r="D3">
+        <v>4.976</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>4.9786666666666664</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="C4">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="D4">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.68299999999999994</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>5.5910000000000002</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>5.7319999999999993</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>5.6619999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>5.6616666666666662</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>2.0999999999999908E-2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>1.000000000000334E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.000000000000334E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>7.6666666666671546E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3.633</v>
+      </c>
+      <c r="C2">
+        <v>3.5630000000000002</v>
+      </c>
+      <c r="D2">
+        <v>3.6960000000000002</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>3.6306666666666665</v>
+      </c>
+      <c r="F2" s="3">
+        <f>('optimized rId in participants'!E2-E2)/'optimized rId in participants'!E2</f>
+        <v>0.3595954844778928</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41811</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3.2410000000000001</v>
+      </c>
+      <c r="C3">
+        <v>3.1850000000000001</v>
+      </c>
+      <c r="D3">
+        <v>3.2890000000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>3.2383333333333333</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.378</v>
+      </c>
+      <c r="D4">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.35433333333333339</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>3.532</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>3.5630000000000002</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.6830000000000003</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5926666666666667</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>0.10099999999999998</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999901E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7999999999999812E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extended batAveCSV to reduce setup time
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="14" activeTab="16"/>
+    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="16" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <sheet name="created c_did_get_hit" sheetId="15" r:id="rId15"/>
     <sheet name="optimized rId in participants" sheetId="16" r:id="rId16"/>
     <sheet name="no redun batAve calcs" sheetId="17" r:id="rId17"/>
+    <sheet name="boxscoreBuffer installed" sheetId="18" r:id="rId18"/>
+    <sheet name="extended batAveCSV" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="26">
   <si>
     <t>T1</t>
   </si>
@@ -101,6 +103,18 @@
   </si>
   <si>
     <t>Dumb.</t>
+  </si>
+  <si>
+    <t>Installed boxscore buffer in cresearcher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added retrosheetID, firstName and lastName to batAveCSV. </t>
+  </si>
+  <si>
+    <t>When we initalize players in setup, we no longer have to</t>
+  </si>
+  <si>
+    <t>recalculate those values.</t>
   </si>
 </sst>
 </file>
@@ -172,8 +186,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -234,7 +252,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -260,6 +278,8 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -285,6 +305,8 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1774,6 +1796,318 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="A1:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3.633</v>
+      </c>
+      <c r="C2">
+        <v>3.5630000000000002</v>
+      </c>
+      <c r="D2">
+        <v>3.6960000000000002</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>3.6306666666666665</v>
+      </c>
+      <c r="F2" s="3">
+        <f>('optimized rId in participants'!E2-E2)/'optimized rId in participants'!E2</f>
+        <v>0.3595954844778928</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41811</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3.2410000000000001</v>
+      </c>
+      <c r="C3">
+        <v>3.1850000000000001</v>
+      </c>
+      <c r="D3">
+        <v>3.2890000000000001</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>3.2383333333333333</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.378</v>
+      </c>
+      <c r="D4">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.35433333333333339</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>3.532</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>3.5630000000000002</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.6830000000000003</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5926666666666667</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>0.10099999999999998</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999901E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7999999999999812E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="A1:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3.1850000000000001</v>
+      </c>
+      <c r="C2">
+        <v>3.1520000000000001</v>
+      </c>
+      <c r="D2">
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>3.170666666666667</v>
+      </c>
+      <c r="F2" s="3">
+        <f>('no redun batAve calcs'!E2-'boxscoreBuffer installed'!E2)/'no redun batAve calcs'!E2</f>
+        <v>0.12669849430774868</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41814</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2.8149999999999999</v>
+      </c>
+      <c r="C3">
+        <v>2.79</v>
+      </c>
+      <c r="D3">
+        <v>2.8079999999999998</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>2.8043333333333336</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.36</v>
+      </c>
+      <c r="D4">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>3.1840000000000002</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>3.15</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.1739999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>3.1693333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>9.9999999999988987E-4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>2.0000000000002238E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>9.9999999999988987E-4</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3333333333336306E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
@@ -1808,24 +2142,24 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3.633</v>
+        <v>1.9019999999999999</v>
       </c>
       <c r="C2">
-        <v>3.5630000000000002</v>
+        <v>1.89</v>
       </c>
       <c r="D2">
-        <v>3.6960000000000002</v>
+        <v>1.9119999999999999</v>
       </c>
       <c r="E2" s="3">
         <f>AVERAGE(B2:D2)</f>
-        <v>3.6306666666666665</v>
+        <v>1.9013333333333333</v>
       </c>
       <c r="F2" s="3">
-        <f>('optimized rId in participants'!E2-E2)/'optimized rId in participants'!E2</f>
-        <v>0.3595954844778928</v>
+        <f>('boxscoreBuffer installed'!E2-'extended batAveCSV'!E2)/'boxscoreBuffer installed'!E2</f>
+        <v>0.40033641715727508</v>
       </c>
       <c r="G2" s="6">
-        <v>41811</v>
+        <v>41814</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
@@ -1836,20 +2170,20 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>3.2410000000000001</v>
+        <v>1.748</v>
       </c>
       <c r="C3">
-        <v>3.1850000000000001</v>
+        <v>1.7390000000000001</v>
       </c>
       <c r="D3">
-        <v>3.2890000000000001</v>
+        <v>1.758</v>
       </c>
       <c r="E3" s="3">
         <f>AVERAGE(B3:D3)</f>
-        <v>3.2383333333333333</v>
+        <v>1.7483333333333333</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1857,20 +2191,20 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.29099999999999998</v>
+        <v>0.153</v>
       </c>
       <c r="C4">
-        <v>0.378</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="D4">
-        <v>0.39400000000000002</v>
+        <v>0.151</v>
       </c>
       <c r="E4" s="3">
         <f>AVERAGE(B4:D4)</f>
-        <v>0.35433333333333339</v>
+        <v>0.151</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1879,22 +2213,22 @@
       </c>
       <c r="B5">
         <f>SUM(B3:B4)</f>
-        <v>3.532</v>
+        <v>1.901</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
-        <v>3.5630000000000002</v>
+        <v>1.8880000000000001</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>3.6830000000000003</v>
+        <v>1.909</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>3.5926666666666667</v>
+        <v>1.8993333333333333</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1903,19 +2237,19 @@
       </c>
       <c r="B6">
         <f>B2-B5</f>
-        <v>0.10099999999999998</v>
+        <v>9.9999999999988987E-4</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:E6" si="1">C2-C5</f>
-        <v>0</v>
+        <v>1.9999999999997797E-3</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>1.2999999999999901E-2</v>
+        <v>2.9999999999998916E-3</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="1"/>
-        <v>3.7999999999999812E-2</v>
+        <v>2.0000000000000018E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get_part_supserset now directly uses a set comprehension
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="17" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="no redun batAve calcs" sheetId="17" r:id="rId17"/>
     <sheet name="boxscoreBuffer installed" sheetId="18" r:id="rId18"/>
     <sheet name="extended batAveCSV" sheetId="19" r:id="rId19"/>
+    <sheet name="optimized get_part_supserset" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="26">
   <si>
     <t>T1</t>
   </si>
@@ -186,8 +187,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -252,7 +255,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -280,6 +283,7 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -307,6 +311,7 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2108,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2254,6 +2259,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2391,6 +2397,164 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1.867</v>
+      </c>
+      <c r="C2">
+        <v>1.8640000000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.873</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>1.8680000000000001</v>
+      </c>
+      <c r="F2" s="3">
+        <f>('extended batAveCSV'!E2-'optimized get_part_supserset'!E2)/'extended batAveCSV'!E2</f>
+        <v>1.7531556802243976E-2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41814</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1.708</v>
+      </c>
+      <c r="C3">
+        <v>1.708</v>
+      </c>
+      <c r="D3">
+        <v>1.72</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>1.712</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.155</v>
+      </c>
+      <c r="C4">
+        <v>0.153</v>
+      </c>
+      <c r="D4">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>0.15233333333333332</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>1.863</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>1.861</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.869</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8643333333333332</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>3.0000000000001137E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>3.666666666666929E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding error handling to C extensions. They all now return python exceptions if an error occurs
</commit_message>
<xml_diff>
--- a/beatthestreak/2010,2009,20,20,D Times.xlsx
+++ b/beatthestreak/2010,2009,20,20,D Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="17" activeTab="19"/>
+    <workbookView xWindow="840" yWindow="0" windowWidth="23460" windowHeight="15380" tabRatio="500" firstSheet="18" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name=" _check_year opt" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="boxscoreBuffer installed" sheetId="18" r:id="rId18"/>
     <sheet name="extended batAveCSV" sheetId="19" r:id="rId19"/>
     <sheet name="optimized get_part_supserset" sheetId="20" r:id="rId20"/>
+    <sheet name="Installed player hit_info hash" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="30">
   <si>
     <t>T1</t>
   </si>
@@ -117,6 +118,18 @@
   <si>
     <t>recalculate those values.</t>
   </si>
+  <si>
+    <t>Installed hash table-based lookup of player hit Infos (hitVals and otherInfo)</t>
+  </si>
+  <si>
+    <t>During setup, csv's of the player's hit info for the entire season</t>
+  </si>
+  <si>
+    <t>are generated, and then lazily loaded into a hash table</t>
+  </si>
+  <si>
+    <t>during the simulation</t>
+  </si>
 </sst>
 </file>
 
@@ -187,8 +200,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -255,7 +270,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -284,6 +299,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -312,6 +328,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2409,8 +2426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2551,6 +2568,168 @@
       <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>3.666666666666929E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1.19</v>
+      </c>
+      <c r="C2">
+        <v>1.222</v>
+      </c>
+      <c r="D2">
+        <v>1.2</v>
+      </c>
+      <c r="E2" s="3">
+        <f>AVERAGE(B2:D2)</f>
+        <v>1.204</v>
+      </c>
+      <c r="F2" s="3">
+        <f>('optimized get_part_supserset'!E2-'Installed player hit_info hash'!E2)/'optimized get_part_supserset'!E2</f>
+        <v>0.35546038543897224</v>
+      </c>
+      <c r="G2" s="6">
+        <v>41814</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1.105</v>
+      </c>
+      <c r="C3">
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="D3">
+        <v>1.113</v>
+      </c>
+      <c r="E3" s="3">
+        <f>AVERAGE(B3:D3)</f>
+        <v>1.1166666666666667</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="C4">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>AVERAGE(B4:D4)</f>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="0">SUM(C3:C4)</f>
+        <v>1.2169999999999999</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.196</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1996666666666667</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <f>B2-B5</f>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="1">C2-C5</f>
+        <v>5.0000000000001155E-3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="1"/>
+        <v>4.3333333333333002E-3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>